<commit_message>
update excel file for plots
minor time adjustments
</commit_message>
<xml_diff>
--- a/data/Cougars_ODBA_Kills_Setup.xlsx
+++ b/data/Cougars_ODBA_Kills_Setup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OSU\AI Capstone\delte\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\binde\Git\ai-capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1874E35-6AD4-42AC-94F8-16B0A0C586D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC8C492-04F3-4C55-9E70-DBD270F5E971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InfoPlots" sheetId="1" r:id="rId1"/>
@@ -4775,7 +4775,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4900,6 +4900,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5304,19 +5305,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M164"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M160" sqref="M160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.5"/>
   <cols>
     <col min="5" max="5" width="10.5" customWidth="1"/>
-    <col min="6" max="6" width="10.296875" customWidth="1"/>
-    <col min="8" max="8" width="12.09765625" customWidth="1"/>
-    <col min="10" max="10" width="13.09765625" customWidth="1"/>
-    <col min="11" max="11" width="16.796875" customWidth="1"/>
-    <col min="12" max="12" width="16.8984375" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.08203125" customWidth="1"/>
+    <col min="10" max="10" width="13.08203125" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" customWidth="1"/>
+    <col min="12" max="12" width="16.9140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -10022,7 +10023,7 @@
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="28" t="s">
@@ -11991,7 +11992,7 @@
       <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:38">
       <c r="A1" s="1" t="s">
@@ -12761,11 +12762,11 @@
   <dimension ref="A1:AN240"/>
   <sheetViews>
     <sheetView zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K129" sqref="K129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="5" max="5" width="8" customWidth="1"/>
   </cols>
@@ -20197,7 +20198,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="97" spans="1:31" ht="31.2">
+    <row r="97" spans="1:31" ht="31">
       <c r="A97" s="2">
         <v>202</v>
       </c>
@@ -20271,7 +20272,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="98" spans="1:31" ht="31.2">
+    <row r="98" spans="1:31" ht="31">
       <c r="A98" s="2">
         <v>202</v>
       </c>
@@ -20345,7 +20346,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="99" spans="1:31" ht="31.2">
+    <row r="99" spans="1:31" ht="31">
       <c r="A99" s="2">
         <v>202</v>
       </c>
@@ -20419,7 +20420,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="100" spans="1:31" ht="31.2">
+    <row r="100" spans="1:31" ht="31">
       <c r="A100" s="2">
         <v>202</v>
       </c>
@@ -22620,7 +22621,7 @@
       <c r="M129" s="5">
         <v>0.83716435185185201</v>
       </c>
-      <c r="N129" s="7">
+      <c r="N129" s="62">
         <v>0.84126157407407398</v>
       </c>
       <c r="O129" s="5">
@@ -30744,9 +30745,9 @@
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.5"/>
   <cols>
-    <col min="8" max="8" width="11.19921875" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -44791,7 +44792,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="197" spans="1:26" ht="31.2">
+    <row r="197" spans="1:26" ht="31">
       <c r="A197" s="2">
         <v>202</v>
       </c>
@@ -44862,7 +44863,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="198" spans="1:26" ht="31.2">
+    <row r="198" spans="1:26" ht="31">
       <c r="A198" s="2">
         <v>202</v>
       </c>
@@ -44933,7 +44934,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="199" spans="1:26" ht="31.2">
+    <row r="199" spans="1:26" ht="31">
       <c r="A199" s="2">
         <v>202</v>
       </c>
@@ -45004,7 +45005,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="200" spans="1:26" ht="31.2">
+    <row r="200" spans="1:26" ht="31">
       <c r="A200" s="2">
         <v>202</v>
       </c>
@@ -66170,9 +66171,9 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="20" max="20" width="26.19921875" customWidth="1"/>
+    <col min="20" max="20" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -69328,7 +69329,7 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" s="1" t="s">
@@ -69389,7 +69390,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="46" customFormat="1" ht="15">
+    <row r="2" spans="1:31" s="46" customFormat="1">
       <c r="A2" s="46">
         <v>202</v>
       </c>
@@ -69445,7 +69446,7 @@
         <v>0.58333333333333304</v>
       </c>
     </row>
-    <row r="3" spans="1:31" s="46" customFormat="1" ht="15">
+    <row r="3" spans="1:31" s="46" customFormat="1">
       <c r="A3" s="46">
         <v>202</v>
       </c>
@@ -69501,7 +69502,7 @@
         <v>0.58333333333333304</v>
       </c>
     </row>
-    <row r="4" spans="1:31" s="46" customFormat="1" ht="15">
+    <row r="4" spans="1:31" s="46" customFormat="1">
       <c r="A4" s="46">
         <v>202</v>
       </c>
@@ -72147,11 +72148,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AM177"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="22" max="22" width="17" customWidth="1"/>
   </cols>
@@ -72286,7 +72287,7 @@
         <v>0.69236111111111098</v>
       </c>
       <c r="N2" s="5">
-        <v>0.69738425925925895</v>
+        <v>0.69739583333333333</v>
       </c>
       <c r="O2" s="5">
         <v>0.69755787037036998</v>
@@ -72424,7 +72425,7 @@
         <v>0.20011574074074101</v>
       </c>
       <c r="O5" s="5">
-        <v>0.20017361111111101</v>
+        <v>0.20018518518518516</v>
       </c>
       <c r="P5" s="5">
         <v>0.20098379629629601</v>
@@ -72688,7 +72689,7 @@
         <v>0.26736111111111099</v>
       </c>
       <c r="M11" s="5">
-        <v>0.26319444444444401</v>
+        <v>0.26041666666666669</v>
       </c>
       <c r="N11" s="7">
         <v>0.26533564814814797</v>
@@ -72829,7 +72830,7 @@
         <v>0.27976851851851797</v>
       </c>
       <c r="O14" s="5">
-        <v>0.28027777777777801</v>
+        <v>0.28028935185185183</v>
       </c>
       <c r="P14" s="5">
         <v>0.28732638888888901</v>
@@ -72838,7 +72839,7 @@
         <v>0.28888888888888897</v>
       </c>
       <c r="R14" s="5">
-        <v>0.29305555555555601</v>
+        <v>0.29930555555555555</v>
       </c>
     </row>
     <row r="15" spans="1:39">
@@ -79556,14 +79557,14 @@
       <selection activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="8" max="8" width="5.796875" customWidth="1"/>
+    <col min="8" max="8" width="5.83203125" customWidth="1"/>
     <col min="9" max="9" width="4" customWidth="1"/>
     <col min="10" max="10" width="7" customWidth="1"/>
-    <col min="14" max="14" width="31.296875" customWidth="1"/>
+    <col min="14" max="14" width="31.33203125" customWidth="1"/>
     <col min="17" max="17" width="39.5" customWidth="1"/>
-    <col min="41" max="41" width="18.69921875" customWidth="1"/>
+    <col min="41" max="41" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43">
@@ -79697,7 +79698,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="2" spans="1:43" s="36" customFormat="1" ht="409.6">
+    <row r="2" spans="1:43" s="36" customFormat="1" ht="403">
       <c r="A2" s="32" t="s">
         <v>722</v>
       </c>
@@ -79928,7 +79929,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Late Winter&lt;br/&gt;825&lt;br/&gt;313&lt;br/&gt;42810</v>
       </c>
     </row>
-    <row r="4" spans="1:43" s="36" customFormat="1" ht="409.6">
+    <row r="4" spans="1:43" s="36" customFormat="1" ht="403">
       <c r="A4" s="32" t="s">
         <v>722</v>
       </c>
@@ -80057,7 +80058,7 @@
         <v>Elk&lt;br/&gt;Male&lt;br/&gt;Polished&lt;br/&gt;Yearling&lt;br/&gt;Late Winter&lt;br/&gt;824&lt;br/&gt;316&lt;br/&gt;42812</v>
       </c>
     </row>
-    <row r="5" spans="1:43" s="36" customFormat="1" ht="327.60000000000002">
+    <row r="5" spans="1:43" s="36" customFormat="1" ht="294.5">
       <c r="A5" s="32" t="s">
         <v>722</v>
       </c>
@@ -80181,7 +80182,7 @@
 &lt;br/&gt;Calf/fawn&lt;br/&gt;Late Winter&lt;br/&gt;852&lt;br/&gt;323&lt;br/&gt;42820</v>
       </c>
     </row>
-    <row r="6" spans="1:43" s="36" customFormat="1" ht="249.6">
+    <row r="6" spans="1:43" s="36" customFormat="1" ht="232.5">
       <c r="A6" s="32" t="s">
         <v>722</v>
       </c>
@@ -80412,7 +80413,7 @@
         <v>Grouse&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Unknown&lt;br/&gt;Summer&lt;br/&gt;855&lt;br/&gt;380&lt;br/&gt;42866</v>
       </c>
     </row>
-    <row r="8" spans="1:43" s="36" customFormat="1" ht="202.8">
+    <row r="8" spans="1:43" s="36" customFormat="1" ht="201.5">
       <c r="A8" s="32" t="s">
         <v>722</v>
       </c>
@@ -80532,7 +80533,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Yearling&lt;br/&gt;Summer&lt;br/&gt;856&lt;br/&gt;387&lt;br/&gt;42872</v>
       </c>
     </row>
-    <row r="9" spans="1:43" s="36" customFormat="1" ht="62.4">
+    <row r="9" spans="1:43" s="36" customFormat="1" ht="62">
       <c r="A9" s="32" t="s">
         <v>722</v>
       </c>
@@ -80622,7 +80623,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Adult&lt;br/&gt;Summer&lt;br/&gt;864&lt;br/&gt;388&lt;br/&gt;42874</v>
       </c>
     </row>
-    <row r="10" spans="1:43" s="36" customFormat="1" ht="31.2">
+    <row r="10" spans="1:43" s="36" customFormat="1" ht="31">
       <c r="A10" s="32" t="s">
         <v>722</v>
       </c>
@@ -80733,7 +80734,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;828&lt;br/&gt;393&lt;br/&gt;42878</v>
       </c>
     </row>
-    <row r="11" spans="1:43" s="36" customFormat="1" ht="156">
+    <row r="11" spans="1:43" s="36" customFormat="1" ht="155">
       <c r="A11" s="32" t="s">
         <v>722</v>
       </c>
@@ -80841,7 +80842,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;871&lt;br/&gt;395&lt;br/&gt;42880</v>
       </c>
     </row>
-    <row r="12" spans="1:43" s="36" customFormat="1" ht="46.8">
+    <row r="12" spans="1:43" s="36" customFormat="1" ht="46.5">
       <c r="A12" s="32" t="s">
         <v>722</v>
       </c>
@@ -80946,7 +80947,7 @@
         <v>Yellow-Bellied Marmot&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Adult&lt;br/&gt;Summer&lt;br/&gt;859&lt;br/&gt;399&lt;br/&gt;42883</v>
       </c>
     </row>
-    <row r="13" spans="1:43" s="36" customFormat="1" ht="409.6">
+    <row r="13" spans="1:43" s="36" customFormat="1" ht="403">
       <c r="A13" s="32" t="s">
         <v>857</v>
       </c>
@@ -81057,7 +81058,7 @@
         <v>Elk&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;865&lt;br/&gt;346&lt;br/&gt;42883</v>
       </c>
     </row>
-    <row r="14" spans="1:43" s="36" customFormat="1" ht="62.4">
+    <row r="14" spans="1:43" s="36" customFormat="1" ht="62">
       <c r="A14" s="32" t="s">
         <v>722</v>
       </c>
@@ -81168,7 +81169,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;869&lt;br/&gt;401&lt;br/&gt;42884</v>
       </c>
     </row>
-    <row r="15" spans="1:43" s="36" customFormat="1" ht="46.8">
+    <row r="15" spans="1:43" s="36" customFormat="1" ht="46.5">
       <c r="A15" s="32" t="s">
         <v>722</v>
       </c>
@@ -81279,7 +81280,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;860&lt;br/&gt;402&lt;br/&gt;42885</v>
       </c>
     </row>
-    <row r="16" spans="1:43" s="36" customFormat="1" ht="358.8">
+    <row r="16" spans="1:43" s="36" customFormat="1" ht="325.5">
       <c r="A16" s="32" t="s">
         <v>722</v>
       </c>
@@ -81390,7 +81391,7 @@
         <v>Elk&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;862&lt;br/&gt;404&lt;br/&gt;42886</v>
       </c>
     </row>
-    <row r="17" spans="1:43" s="36" customFormat="1" ht="78">
+    <row r="17" spans="1:43" s="36" customFormat="1" ht="77.5">
       <c r="A17" s="32" t="s">
         <v>722</v>
       </c>
@@ -81498,7 +81499,7 @@
         <v>Pronghorn Antelope&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;861&lt;br/&gt;406&lt;br/&gt;42888</v>
       </c>
     </row>
-    <row r="18" spans="1:43" s="36" customFormat="1" ht="171.6">
+    <row r="18" spans="1:43" s="36" customFormat="1" ht="139.5">
       <c r="A18" s="32" t="s">
         <v>722</v>
       </c>
@@ -81615,7 +81616,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;863&lt;br/&gt;404&lt;br/&gt;42889</v>
       </c>
     </row>
-    <row r="19" spans="1:43" s="36" customFormat="1" ht="265.2">
+    <row r="19" spans="1:43" s="36" customFormat="1" ht="232.5">
       <c r="A19" s="32" t="s">
         <v>722</v>
       </c>
@@ -81717,7 +81718,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;867&lt;br/&gt;409&lt;br/&gt;42891</v>
       </c>
     </row>
-    <row r="20" spans="1:43" s="36" customFormat="1" ht="140.4">
+    <row r="20" spans="1:43" s="36" customFormat="1" ht="124">
       <c r="A20" s="32" t="s">
         <v>722</v>
       </c>
@@ -81825,7 +81826,7 @@
         <v>Elk&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;870&lt;br/&gt;411&lt;br/&gt;42892</v>
       </c>
     </row>
-    <row r="21" spans="1:43" s="36" customFormat="1" ht="409.6">
+    <row r="21" spans="1:43" s="36" customFormat="1" ht="387.5">
       <c r="A21" s="32" t="s">
         <v>722</v>
       </c>
@@ -81942,7 +81943,7 @@
         <v>Pronghorn Antelope&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Adult&lt;br/&gt;Summer&lt;br/&gt;868&lt;br/&gt;415&lt;br/&gt;42894</v>
       </c>
     </row>
-    <row r="22" spans="1:43" s="36" customFormat="1" ht="409.6">
+    <row r="22" spans="1:43" s="36" customFormat="1" ht="403">
       <c r="A22" s="32" t="s">
         <v>722</v>
       </c>
@@ -82062,7 +82063,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Adult&lt;br/&gt;Summer&lt;br/&gt;874&lt;br/&gt;419&lt;br/&gt;42899</v>
       </c>
     </row>
-    <row r="23" spans="1:43" s="36" customFormat="1" ht="234">
+    <row r="23" spans="1:43" s="36" customFormat="1" ht="232.5">
       <c r="A23" s="32" t="s">
         <v>722</v>
       </c>
@@ -82503,7 +82504,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;831&lt;br/&gt;431&lt;br/&gt;42907</v>
       </c>
     </row>
-    <row r="27" spans="1:43" s="36" customFormat="1" ht="409.6">
+    <row r="27" spans="1:43" s="36" customFormat="1" ht="387.5">
       <c r="A27" s="32" t="s">
         <v>722</v>
       </c>
@@ -82725,7 +82726,7 @@
         <v>Grouse&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Unknown&lt;br/&gt;Summer&lt;br/&gt;883&lt;br/&gt;451&lt;br/&gt;42918</v>
       </c>
     </row>
-    <row r="29" spans="1:43" s="36" customFormat="1" ht="46.8">
+    <row r="29" spans="1:43" s="36" customFormat="1" ht="31">
       <c r="A29" s="32" t="s">
         <v>722</v>
       </c>
@@ -82833,7 +82834,7 @@
         <v>Pronghorn Antelope&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;884&lt;br/&gt;453&lt;br/&gt;42918</v>
       </c>
     </row>
-    <row r="30" spans="1:43" s="36" customFormat="1" ht="187.2">
+    <row r="30" spans="1:43" s="36" customFormat="1" ht="170.5">
       <c r="A30" s="32" t="s">
         <v>722</v>
       </c>
@@ -82950,7 +82951,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;837&lt;br/&gt;454&lt;br/&gt;42920</v>
       </c>
     </row>
-    <row r="31" spans="1:43" s="36" customFormat="1" ht="280.8">
+    <row r="31" spans="1:43" s="36" customFormat="1" ht="248">
       <c r="A31" s="32" t="s">
         <v>722</v>
       </c>
@@ -83052,7 +83053,7 @@
         <v>Elk&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;886&lt;br/&gt;460&lt;br/&gt;42924</v>
       </c>
     </row>
-    <row r="32" spans="1:43" s="36" customFormat="1" ht="374.4">
+    <row r="32" spans="1:43" s="36" customFormat="1" ht="341">
       <c r="A32" s="32" t="s">
         <v>722</v>
       </c>
@@ -83160,7 +83161,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Adult&lt;br/&gt;Summer&lt;br/&gt;885&lt;br/&gt;462&lt;br/&gt;42925</v>
       </c>
     </row>
-    <row r="33" spans="1:43" s="36" customFormat="1" ht="46.8">
+    <row r="33" spans="1:43" s="36" customFormat="1" ht="46.5">
       <c r="A33" s="32" t="s">
         <v>722</v>
       </c>
@@ -83271,7 +83272,7 @@
         <v>Pronghorn Antelope&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;838&lt;br/&gt;466&lt;br/&gt;42929</v>
       </c>
     </row>
-    <row r="34" spans="1:43" s="36" customFormat="1" ht="124.8">
+    <row r="34" spans="1:43" s="36" customFormat="1" ht="124">
       <c r="A34" s="32" t="s">
         <v>722</v>
       </c>
@@ -83379,7 +83380,7 @@
         <v>Pronghorn Antelope&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;892&lt;br/&gt;471&lt;br/&gt;42931</v>
       </c>
     </row>
-    <row r="35" spans="1:43" s="36" customFormat="1" ht="109.2">
+    <row r="35" spans="1:43" s="36" customFormat="1" ht="108.5">
       <c r="A35" s="32" t="s">
         <v>722</v>
       </c>
@@ -83490,7 +83491,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;836&lt;br/&gt;474&lt;br/&gt;42934</v>
       </c>
     </row>
-    <row r="36" spans="1:43" s="36" customFormat="1" ht="409.6">
+    <row r="36" spans="1:43" s="36" customFormat="1" ht="387.5">
       <c r="A36" s="32" t="s">
         <v>722</v>
       </c>
@@ -83613,7 +83614,7 @@
         <v>Elk&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Old adult (10+ yrs)&lt;br/&gt;Summer&lt;br/&gt;835&lt;br/&gt;476&lt;br/&gt;42935</v>
       </c>
     </row>
-    <row r="37" spans="1:43" s="45" customFormat="1" ht="171.6">
+    <row r="37" spans="1:43" s="45" customFormat="1" ht="155">
       <c r="A37" s="41" t="s">
         <v>722</v>
       </c>
@@ -83850,7 +83851,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Yearling&lt;br/&gt;Early Winter&lt;br/&gt;229&lt;br/&gt;215&lt;br/&gt;43054</v>
       </c>
     </row>
-    <row r="39" spans="1:43" s="36" customFormat="1" ht="327.60000000000002">
+    <row r="39" spans="1:43" s="36" customFormat="1" ht="294.5">
       <c r="A39" s="32" t="s">
         <v>722</v>
       </c>
@@ -83964,7 +83965,7 @@
         <v>Coyote&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Adult&lt;br/&gt;Early Winter&lt;br/&gt;228&lt;br/&gt;218&lt;br/&gt;43058</v>
       </c>
     </row>
-    <row r="40" spans="1:43" s="36" customFormat="1" ht="202.8">
+    <row r="40" spans="1:43" s="36" customFormat="1" ht="186">
       <c r="A40" s="32" t="s">
         <v>722</v>
       </c>
@@ -84087,7 +84088,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Adult&lt;br/&gt;Early Winter&lt;br/&gt;230&lt;br/&gt;230&lt;br/&gt;43067</v>
       </c>
     </row>
-    <row r="41" spans="1:43" s="36" customFormat="1" ht="62.4">
+    <row r="41" spans="1:43" s="36" customFormat="1" ht="62">
       <c r="A41" s="32" t="s">
         <v>722</v>
       </c>
@@ -84207,7 +84208,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Early Winter&lt;br/&gt;231&lt;br/&gt;233&lt;br/&gt;43070</v>
       </c>
     </row>
-    <row r="42" spans="1:43" s="36" customFormat="1" ht="78">
+    <row r="42" spans="1:43" s="36" customFormat="1" ht="77.5">
       <c r="A42" s="32" t="s">
         <v>722</v>
       </c>
@@ -84438,7 +84439,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Early Winter&lt;br/&gt;234&lt;br/&gt;241&lt;br/&gt;43083</v>
       </c>
     </row>
-    <row r="44" spans="1:43" s="36" customFormat="1" ht="327.60000000000002">
+    <row r="44" spans="1:43" s="36" customFormat="1" ht="294.5">
       <c r="A44" s="32" t="s">
         <v>722</v>
       </c>
@@ -84544,7 +84545,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Late Winter&lt;br/&gt;943&lt;br/&gt;&lt;br/&gt;43151</v>
       </c>
     </row>
-    <row r="45" spans="1:43" s="36" customFormat="1" ht="109.2">
+    <row r="45" spans="1:43" s="36" customFormat="1" ht="108.5">
       <c r="A45" s="32" t="s">
         <v>722</v>
       </c>
@@ -84650,7 +84651,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Late Winter&lt;br/&gt;953&lt;br/&gt;&lt;br/&gt;43157</v>
       </c>
     </row>
-    <row r="46" spans="1:43" s="36" customFormat="1" ht="358.8">
+    <row r="46" spans="1:43" s="36" customFormat="1" ht="325.5">
       <c r="A46" s="32" t="s">
         <v>722</v>
       </c>
@@ -84747,7 +84748,7 @@
         <v>Red Fox&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Adult&lt;br/&gt;Late Winter&lt;br/&gt;952&lt;br/&gt;&lt;br/&gt;43162</v>
       </c>
     </row>
-    <row r="47" spans="1:43" s="36" customFormat="1" ht="409.6">
+    <row r="47" spans="1:43" s="36" customFormat="1" ht="403">
       <c r="A47" s="32" t="s">
         <v>722</v>
       </c>
@@ -84853,7 +84854,7 @@
         <v>Elk&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Old adult (10+ yrs)&lt;br/&gt;Late Winter&lt;br/&gt;961&lt;br/&gt;&lt;br/&gt;43163</v>
       </c>
     </row>
-    <row r="48" spans="1:43" s="45" customFormat="1" ht="409.6">
+    <row r="48" spans="1:43" s="45" customFormat="1" ht="403">
       <c r="A48" s="41" t="s">
         <v>722</v>
       </c>
@@ -84965,7 +84966,7 @@
         <v>Elk&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Old adult (10+ yrs)&lt;br/&gt;Late Winter&lt;br/&gt;938&lt;br/&gt;&lt;br/&gt;43143</v>
       </c>
     </row>
-    <row r="49" spans="1:45" s="36" customFormat="1" ht="405.6">
+    <row r="49" spans="1:45" s="36" customFormat="1" ht="372">
       <c r="A49" s="32" t="s">
         <v>722</v>
       </c>
@@ -85065,7 +85066,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Late Winter&lt;br/&gt;967&lt;br/&gt;&lt;br/&gt;43173</v>
       </c>
     </row>
-    <row r="50" spans="1:45" ht="409.6">
+    <row r="50" spans="1:45" ht="403">
       <c r="A50" s="23" t="s">
         <v>722</v>
       </c>
@@ -85174,7 +85175,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Late Winter&lt;br/&gt;939&lt;br/&gt;&lt;br/&gt;43177</v>
       </c>
     </row>
-    <row r="51" spans="1:45" s="36" customFormat="1" ht="358.8">
+    <row r="51" spans="1:45" s="36" customFormat="1" ht="325.5">
       <c r="A51" s="32" t="s">
         <v>722</v>
       </c>
@@ -85280,7 +85281,7 @@
         <v>Elk&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Late Winter&lt;br/&gt;969&lt;br/&gt;&lt;br/&gt;43178</v>
       </c>
     </row>
-    <row r="52" spans="1:45" ht="409.6">
+    <row r="52" spans="1:45" ht="387.5">
       <c r="A52" s="23" t="s">
         <v>722</v>
       </c>
@@ -85517,7 +85518,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="55" spans="1:45" s="36" customFormat="1" ht="409.6">
+    <row r="55" spans="1:45" s="36" customFormat="1" ht="409.5">
       <c r="A55" s="31">
         <v>18</v>
       </c>
@@ -85624,7 +85625,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="56" spans="1:45" s="36" customFormat="1" ht="156">
+    <row r="56" spans="1:45" s="36" customFormat="1" ht="155">
       <c r="A56" s="31">
         <v>24</v>
       </c>
@@ -85731,7 +85732,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="57" spans="1:45" s="36" customFormat="1" ht="409.6">
+    <row r="57" spans="1:45" s="36" customFormat="1" ht="403">
       <c r="A57" s="31">
         <v>27</v>
       </c>
@@ -86266,7 +86267,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="62" spans="1:45" ht="409.6">
+    <row r="62" spans="1:45" ht="409.5">
       <c r="A62" s="3">
         <v>51</v>
       </c>
@@ -86384,10 +86385,10 @@
   <dimension ref="A1:AL70"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:38">
       <c r="A1" s="1" t="s">
@@ -86645,10 +86646,10 @@
         <v>0.23888888888888901</v>
       </c>
       <c r="L5" s="5">
-        <v>0.235416666666667</v>
+        <v>0.23541666666666669</v>
       </c>
       <c r="M5" s="5">
-        <v>0.239050925925926</v>
+        <v>0.23906249999999998</v>
       </c>
       <c r="N5" s="5">
         <v>0.23944444444444399</v>
@@ -86739,7 +86740,7 @@
         <v>0.42638888888888898</v>
       </c>
       <c r="L7" s="5">
-        <v>0.41875000000000001</v>
+        <v>0.41944444444444445</v>
       </c>
       <c r="M7" s="5">
         <v>0.42700231481481499</v>

</xml_diff>